<commit_message>
Additions in the file with the texts
</commit_message>
<xml_diff>
--- a/files/texts.xlsx
+++ b/files/texts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PROJECTS\MusicModeForYoutubePrivate\MusicModeForYoutube\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PROJECTS\MusicModeForYouTubeMiscellaneous\TEXTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56D0C05C-07B0-4512-A2B0-BBF219597B4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9119D753-EFD8-4F1E-8F23-A4FD2F12F524}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="INSTRUCTIONS" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="109">
   <si>
     <t>Blocks the video keeping only the audio on YouTube and YouTube Music.</t>
   </si>
@@ -105,9 +105,6 @@
     <t>Developer: Nick Pantelidis</t>
   </si>
   <si>
-    <t>For problems or suggestions, please contact me via email or at the Chrome Web Store.If you wish to contribute translating the extension in another language, please contact me via email</t>
-  </si>
-  <si>
     <t>Current tab</t>
   </si>
   <si>
@@ -340,6 +337,18 @@
   </si>
   <si>
     <t>Words that in your language they may be used as they are (e.g ok, on, off), leave them as they are</t>
+  </si>
+  <si>
+    <t>For problems or suggestions, please contact me via email or at the Chrome Web Store</t>
+  </si>
+  <si>
+    <t>Hide images</t>
+  </si>
+  <si>
+    <t>Show images</t>
+  </si>
+  <si>
+    <t>Translated by Thunderarea</t>
   </si>
 </sst>
 </file>
@@ -355,7 +364,8 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
-      <charset val="1"/>
+      <family val="2"/>
+      <charset val="161"/>
     </font>
     <font>
       <b/>
@@ -764,7 +774,7 @@
   </sheetPr>
   <dimension ref="A1:B56"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
@@ -776,18 +786,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B1" s="3"/>
     </row>
     <row r="2" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15" x14ac:dyDescent="0.25">
@@ -795,7 +805,7 @@
     </row>
     <row r="5" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
@@ -820,10 +830,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B78"/>
+  <dimension ref="A1:B81"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -834,15 +844,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>98</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -852,7 +862,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -949,77 +959,77 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B23" s="2"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B24" s="2"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B25" s="2"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B26" s="2"/>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B27" s="2"/>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
@@ -1027,27 +1037,27 @@
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
@@ -1067,148 +1077,163 @@
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49" s="4" t="s">
-        <v>31</v>
+      <c r="A49" s="1" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50" s="1" t="s">
-        <v>70</v>
+      <c r="A50" s="4" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A51" s="4" t="s">
-        <v>74</v>
+      <c r="A51" s="1" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A55" s="1" t="s">
-        <v>62</v>
+      <c r="A55" s="4" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A64" s="7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" s="7" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" ht="145.19999999999999" x14ac:dyDescent="0.25">
+      <c r="A66" s="4" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="65" spans="1:1" ht="145.19999999999999" x14ac:dyDescent="0.25">
-      <c r="A65" s="4" t="s">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" s="7" t="s">
         <v>85</v>
-      </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A67" s="7" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A68" s="1" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A70" s="1"/>
+      <c r="A70" s="1" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A71" s="7" t="s">
-        <v>88</v>
+      <c r="A71" s="1" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A72" s="4" t="s">
+      <c r="A72" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" s="1"/>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" s="7" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A73" s="4" t="s">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A74" s="4" t="s">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A75" s="4"/>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A76" s="1"/>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A77" s="1"/>
-    </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A78" s="1"/>
+      <c r="A78" s="4"/>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" s="1"/>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" s="1"/>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1219,8 +1244,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B34"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1231,118 +1256,118 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>98</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="66" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="17" spans="1:1" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="19" spans="1:1" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="21" spans="1:1" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
@@ -1350,9 +1375,9 @@
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="1:1" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>27</v>
+        <v>105</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
@@ -1360,7 +1385,7 @@
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
@@ -1370,27 +1395,27 @@
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New file with texts
</commit_message>
<xml_diff>
--- a/files/texts.xlsx
+++ b/files/texts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PROJECTS\MusicModeForYouTubeMiscellaneous\TEXTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9119D753-EFD8-4F1E-8F23-A4FD2F12F524}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1A6E229-A6A8-43B2-8405-1CCAC3BCD909}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="INSTRUCTIONS" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="110">
   <si>
     <t>Blocks the video keeping only the audio on YouTube and YouTube Music.</t>
   </si>
@@ -349,6 +349,9 @@
   </si>
   <si>
     <t>Translated by Thunderarea</t>
+  </si>
+  <si>
+    <t>Follow</t>
   </si>
 </sst>
 </file>
@@ -830,9 +833,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B81"/>
+  <dimension ref="A1:B82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+    <sheetView topLeftCell="A67" workbookViewId="0">
       <selection activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
@@ -1087,153 +1090,158 @@
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>71</v>
+        <v>109</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50" s="4" t="s">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" s="4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A51" s="1" t="s">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
         <v>69</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A52" s="4" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" s="4" t="s">
         <v>76</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A56" s="1" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A65" s="7" t="s">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" s="7" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="66" spans="1:1" ht="145.19999999999999" x14ac:dyDescent="0.25">
-      <c r="A66" s="4" t="s">
+    <row r="67" spans="1:1" ht="145.19999999999999" x14ac:dyDescent="0.25">
+      <c r="A67" s="4" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A68" s="7" t="s">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" s="7" t="s">
         <v>85</v>
-      </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A69" s="1" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>106</v>
+        <v>55</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A73" s="1"/>
-    </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A74" s="7" t="s">
+      <c r="A74" s="1"/>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" s="7" t="s">
         <v>87</v>
-      </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A75" s="4" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" s="4" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A78" s="4"/>
-    </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A79" s="1"/>
+      <c r="A79" s="4"/>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" s="1"/>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" s="1"/>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1244,7 +1252,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B34"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>

</xml_diff>